<commit_message>
Updated file extensions list
</commit_message>
<xml_diff>
--- a/Reference Docs/File Extensions.xlsx
+++ b/Reference Docs/File Extensions.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rakans\Documents\Sierra\Projects\File Exchange\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{793A229D-7F97-4A87-A7F1-A12FEACF889B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
   <si>
     <t>Table 1</t>
   </si>
@@ -107,9 +115,6 @@
     <t>.drd</t>
   </si>
   <si>
-    <t>thruhole.tap</t>
-  </si>
-  <si>
     <t>Board Outline</t>
   </si>
   <si>
@@ -119,9 +124,6 @@
     <t>.gko</t>
   </si>
   <si>
-    <t>Internal Layers</t>
-  </si>
-  <si>
     <t>.gp1</t>
   </si>
   <si>
@@ -135,15 +137,99 @@
   </si>
   <si>
     <t>Readme</t>
+  </si>
+  <si>
+    <t>Top Paste</t>
+  </si>
+  <si>
+    <t>.gtp</t>
+  </si>
+  <si>
+    <t>Bot Paste</t>
+  </si>
+  <si>
+    <t>.gbp</t>
+  </si>
+  <si>
+    <t>Internal Plane Layers</t>
+  </si>
+  <si>
+    <t>.gm#, .gd#, .gg#</t>
+  </si>
+  <si>
+    <t>EIA NC Drill File</t>
+  </si>
+  <si>
+    <t>.drl</t>
+  </si>
+  <si>
+    <t>Internal Signal Layers</t>
+  </si>
+  <si>
+    <t>EAGLE CAM Processor 8.2.2</t>
+  </si>
+  <si>
+    <t>.gbm</t>
+  </si>
+  <si>
+    <t>Gerber Drawings</t>
+  </si>
+  <si>
+    <t>.gtd</t>
+  </si>
+  <si>
+    <t>.gtm</t>
+  </si>
+  <si>
+    <t>.drd, .txt</t>
+  </si>
+  <si>
+    <t>CAMtastic7</t>
+  </si>
+  <si>
+    <t>.gm#</t>
+  </si>
+  <si>
+    <t>.crc</t>
+  </si>
+  <si>
+    <t>.crs</t>
+  </si>
+  <si>
+    <t>eagle version=7.6.0</t>
+  </si>
+  <si>
+    <t>.dim</t>
+  </si>
+  <si>
+    <t>.i#</t>
+  </si>
+  <si>
+    <t>.spt</t>
+  </si>
+  <si>
+    <t>.bol</t>
+  </si>
+  <si>
+    <t>in#</t>
+  </si>
+  <si>
+    <t>.in#</t>
+  </si>
+  <si>
+    <t>.spb</t>
+  </si>
+  <si>
+    <t>.drd, .asb, .ast, .fab</t>
+  </si>
+  <si>
+    <t>thruhole.tap, .tap, .npt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -156,7 +242,7 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -167,7 +253,7 @@
       <name val="Helvetica Neue Medium"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,12 +269,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -308,61 +388,70 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -372,27 +461,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ff1db000"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FF1DB000"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -591,7 +738,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -610,7 +757,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -640,7 +787,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -666,7 +813,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -692,7 +839,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -718,7 +865,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -744,7 +891,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -770,7 +917,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -796,7 +943,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -822,7 +969,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -848,7 +995,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -861,9 +1008,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -880,7 +1033,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -899,7 +1052,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -925,7 +1078,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -951,7 +1104,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -977,7 +1130,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1003,7 +1156,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1029,7 +1182,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1055,7 +1208,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1081,7 +1234,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1107,7 +1260,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1133,7 +1286,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1146,9 +1299,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1162,7 +1321,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1181,7 +1340,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1211,7 +1370,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1237,7 +1396,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1263,7 +1422,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1289,7 +1448,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1315,7 +1474,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1341,7 +1500,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1367,7 +1526,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1393,7 +1552,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1419,7 +1578,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1432,338 +1591,447 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G23"/>
+  <dimension ref="A1:IV23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.265625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35" style="1" customWidth="1"/>
+    <col min="2" max="3" width="16.265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1328125" style="1" customWidth="1"/>
+    <col min="6" max="256" width="16.265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" t="s" s="5">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+    </row>
+    <row r="2" spans="1:7" ht="20.25" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="33.75" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" ht="34.7" customHeight="1">
-      <c r="A4" t="s" s="8">
+      <c r="E3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="34.700000000000003" customHeight="1">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s" s="9">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s" s="10">
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="10">
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="8">
+      <c r="E4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="12">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="13">
+      <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s" s="13">
+      <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="8">
+      <c r="E5" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s" s="12">
+      <c r="B6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s" s="13">
+      <c r="C6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s" s="13">
+      <c r="D6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="8">
+      <c r="E6" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s" s="12">
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s" s="13">
+      <c r="C7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s" s="13">
+      <c r="D7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="14">
+      <c r="E7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13.15">
+      <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s" s="12">
+      <c r="B8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s" s="13">
+      <c r="C8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s" s="13">
+      <c r="D8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="8">
+      <c r="E8" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="13.15">
+      <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s" s="12">
+      <c r="B9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s" s="13">
+      <c r="C9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="s" s="13">
+      <c r="D9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="8">
+      <c r="E9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s" s="12">
+      <c r="B10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s" s="13">
+      <c r="C10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s" s="13">
+      <c r="D10" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="8">
+      <c r="B11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s" s="12">
+      <c r="C11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C11" t="s" s="13">
+      <c r="D11" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="8">
+      <c r="C12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" t="s" s="12">
+      <c r="D12" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s" s="13">
+      <c r="B13" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="8">
+      <c r="C13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s" s="12">
+      <c r="B14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C13" t="s" s="13">
-        <v>39</v>
-      </c>
-      <c r="D13" t="s" s="13">
-        <v>39</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="8">
+      <c r="B15" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s" s="12">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s" s="13">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s" s="13">
-        <v>29</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
design for extensionFile and cassandra method for filetypeId
</commit_message>
<xml_diff>
--- a/Reference Docs/File Extensions.xlsx
+++ b/Reference Docs/File Extensions.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr date1904="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rakans\Documents\Sierra\Projects\File Exchange\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{793A229D-7F97-4A87-A7F1-A12FEACF889B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -220,17 +214,39 @@
     <t>.spb</t>
   </si>
   <si>
-    <t>.drd, .asb, .ast, .fab</t>
-  </si>
-  <si>
-    <t>thruhole.tap, .tap, .npt</t>
+    <r>
+      <t xml:space="preserve">thruhole.tap, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>.tap, .npt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">.drd, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>.asb, .ast, .fab</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -251,6 +267,19 @@
       <sz val="22"/>
       <color indexed="8"/>
       <name val="Helvetica Neue Medium"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="4">
@@ -392,7 +421,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -452,6 +481,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1609,7 +1644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1619,16 +1654,19 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.265625" defaultRowHeight="19.899999999999999" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="35" style="1" customWidth="1"/>
-    <col min="2" max="3" width="16.265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.59765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1328125" style="1" customWidth="1"/>
-    <col min="6" max="256" width="16.265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" style="1" customWidth="1"/>
+    <col min="8" max="256" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1">
@@ -1708,7 +1746,7 @@
       <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="20" t="s">
         <v>52</v>
       </c>
       <c r="F5" s="16" t="s">
@@ -1764,7 +1802,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.15">
+    <row r="8" spans="1:7" ht="15">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1777,7 +1815,7 @@
       <c r="D8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="20" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="16" t="s">
@@ -1787,7 +1825,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="13.15">
+    <row r="9" spans="1:7" ht="12.75">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1819,7 +1857,7 @@
         <v>30</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>53</v>
@@ -1839,14 +1877,14 @@
       <c r="C11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="20" t="s">
         <v>62</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="10"/>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="20" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1860,12 +1898,12 @@
       <c r="C12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="20" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="20" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1907,20 +1945,20 @@
       <c r="A15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="20" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="16"/>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="20" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1928,18 +1966,18 @@
       <c r="A16" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="20" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="16"/>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="14" t="s">
         <v>42</v>
       </c>
       <c r="F16" s="10"/>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="20" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1962,17 +2000,17 @@
       <c r="A18" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="21" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="20" t="s">
         <v>55</v>
       </c>
       <c r="G18" s="10"/>
@@ -1981,7 +2019,7 @@
       <c r="A19" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="20" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="10"/>
@@ -2031,7 +2069,7 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>